<commit_message>
Segunda revision de la matriz
</commit_message>
<xml_diff>
--- a/Archivos/reporte_stock.xlsx
+++ b/Archivos/reporte_stock.xlsx
@@ -469,10 +469,8 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="E2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3">

</xml_diff>